<commit_message>
Prova non funzionante di resnet50
</commit_message>
<xml_diff>
--- a/Analisi sintetica dei dati.xlsx
+++ b/Analisi sintetica dei dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauroloddo/Documents/MATLAB/SeedClasification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E4F788-19C3-4C44-A201-B06894DE7BFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC04CA7-8B9F-184B-8399-A4F81BDEC9FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" xr2:uid="{E3CBB1D1-38F6-D048-9B05-7C344C0DC1BE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Classificazione</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>dati dalla media di 5 test per rete</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,15 +750,15 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="18"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
@@ -764,15 +767,33 @@
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="A7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="24" t="s">
@@ -785,15 +806,27 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="A8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="20">
+        <v>20</v>
+      </c>
+      <c r="D8" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E8" s="20">
+        <v>64</v>
+      </c>
+      <c r="F8" s="20">
+        <v>5</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="18"/>
       <c r="K8" s="20"/>
       <c r="L8" s="24" t="s">
@@ -806,15 +839,6 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
       <c r="J9" s="18"/>
       <c r="K9" s="20"/>
       <c r="L9" s="24" t="s">

</xml_diff>

<commit_message>
Finite analisi con resnet
</commit_message>
<xml_diff>
--- a/Analisi sintetica dei dati.xlsx
+++ b/Analisi sintetica dei dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauroloddo/Documents/MATLAB/SeedClasification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC04CA7-8B9F-184B-8399-A4F81BDEC9FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC7BE90-0F59-B144-B302-91449A228EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" xr2:uid="{E3CBB1D1-38F6-D048-9B05-7C344C0DC1BE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Classificazione</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>ResNet50</t>
+  </si>
+  <si>
+    <t>ResNet18</t>
+  </si>
+  <si>
+    <t>ResNet101</t>
   </si>
 </sst>
 </file>
@@ -594,7 +600,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -824,9 +830,15 @@
       <c r="F8" s="20">
         <v>5</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
+      <c r="G8" s="22">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0.96279999999999999</v>
+      </c>
       <c r="J8" s="18"/>
       <c r="K8" s="20"/>
       <c r="L8" s="24" t="s">
@@ -839,6 +851,15 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="18"/>
       <c r="K9" s="20"/>
       <c r="L9" s="24" t="s">
@@ -851,15 +872,33 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="J10" s="18"/>
       <c r="K10" s="20"/>
       <c r="L10" s="18"/>
@@ -868,15 +907,33 @@
       <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="20">
+        <v>20</v>
+      </c>
+      <c r="D11" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E11" s="20">
+        <v>64</v>
+      </c>
+      <c r="F11" s="20">
+        <v>5</v>
+      </c>
+      <c r="G11" s="22">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0.96879999999999999</v>
+      </c>
       <c r="J11" s="18"/>
       <c r="K11" s="20"/>
       <c r="L11" s="26" t="s">
@@ -887,15 +944,15 @@
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="28" t="s">
@@ -906,28 +963,64 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="A13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="A14" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="20">
+        <v>20</v>
+      </c>
+      <c r="D14" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E14" s="20">
+        <v>64</v>
+      </c>
+      <c r="F14" s="20">
+        <v>5</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.96819999999999995</v>
+      </c>
+      <c r="I14" s="23">
+        <v>0.96889999999999998</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="4"/>
     </row>

</xml_diff>

<commit_message>
Piccole modifiche per prestazioni migliori
</commit_message>
<xml_diff>
--- a/Analisi sintetica dei dati.xlsx
+++ b/Analisi sintetica dei dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauroloddo/Documents/MATLAB/SeedClasification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7585FB-DB6E-FB4E-B45C-775CBA1FABF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78264B5-73B9-7146-9A4A-A22420D5859D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" xr2:uid="{E3CBB1D1-38F6-D048-9B05-7C344C0DC1BE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="31">
   <si>
     <t>Classificazione</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>InceptionV3</t>
-  </si>
-  <si>
-    <t>Risultati davvero bassi con tempi di lavoro molto lunghi</t>
   </si>
   <si>
     <t>VGG16</t>
@@ -618,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966282BA-1F9E-5348-BB55-D0E2FD507CE7}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,9 +1298,6 @@
       <c r="I25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J25" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
@@ -1313,7 +1307,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="20">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D26" s="21">
         <v>1E-4</v>
@@ -1324,9 +1318,15 @@
       <c r="F26" s="20">
         <v>5</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="G26" s="22">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0.98080000000000001</v>
+      </c>
+      <c r="I26" s="23">
+        <v>0.97330000000000005</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>14</v>
@@ -1464,6 +1464,202 @@
       </c>
       <c r="I32" s="23">
         <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="20">
+        <v>80</v>
+      </c>
+      <c r="D41" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E41" s="20">
+        <v>64</v>
+      </c>
+      <c r="F41" s="20">
+        <v>5</v>
+      </c>
+      <c r="G41" s="22">
+        <v>0.94779999999999998</v>
+      </c>
+      <c r="H41" s="23">
+        <v>0.95479999999999998</v>
+      </c>
+      <c r="I41" s="23">
+        <v>0.94330000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="20">
+        <v>100</v>
+      </c>
+      <c r="D44" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E44" s="20">
+        <v>64</v>
+      </c>
+      <c r="F44" s="20">
+        <v>5</v>
+      </c>
+      <c r="G44" s="22">
+        <v>0.97389999999999999</v>
+      </c>
+      <c r="H44" s="23">
+        <v>0.98209999999999997</v>
+      </c>
+      <c r="I44" s="23">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="20">
+        <v>100</v>
+      </c>
+      <c r="D47" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="E47" s="20">
+        <v>64</v>
+      </c>
+      <c r="F47" s="20">
+        <v>5</v>
+      </c>
+      <c r="G47" s="22">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="H47" s="23">
+        <v>0.9788</v>
+      </c>
+      <c r="I47" s="23">
+        <v>0.96989999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VGG16 con 100 epoche
</commit_message>
<xml_diff>
--- a/Analisi sintetica dei dati.xlsx
+++ b/Analisi sintetica dei dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauroloddo/Documents/MATLAB/SeedClasification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88BC2D5-D491-D146-A726-0C9F76FB8DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6B9C41-FC47-1E4A-9764-19BA563EE777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" xr2:uid="{E3CBB1D1-38F6-D048-9B05-7C344C0DC1BE}"/>
   </bookViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966282BA-1F9E-5348-BB55-D0E2FD507CE7}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1721,9 +1721,15 @@
       <c r="F50" s="20">
         <v>5</v>
       </c>
-      <c r="G50" s="22"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
+      <c r="G50" s="22">
+        <v>0.86950000000000005</v>
+      </c>
+      <c r="H50" s="23">
+        <v>0.88870000000000005</v>
+      </c>
+      <c r="I50" s="23">
+        <v>0.88329999999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>